<commit_message>
Conversion to .csv and .py
</commit_message>
<xml_diff>
--- a/Compressor performance converted.xlsx
+++ b/Compressor performance converted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/230cc5a23d7a19aa/Documents/GitHub/Compression-Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3A5A8F-6B59-48C3-8171-CA4B49D17136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3F3A5A8F-6B59-48C3-8171-CA4B49D17136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B29E841B-ECB3-4EA8-9F7C-A15E2E507976}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="360">
   <si>
     <t/>
   </si>
@@ -1615,7 +1615,7 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:L1"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1892,9 +1892,6 @@
       <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
       <c r="E10" t="s">
         <v>0</v>
       </c>
@@ -3563,7 +3560,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C2:L2 C12:L12 D3:L4 C10:L10 D11:L11 C14:L15 D13:L13 C19:L19 D18:L18 C61:L61 D20:L20 C21:L22 C26:L26 C33:L33 C40:L40 C47:L47 C54:L54 D25:L25 C28:L29 D27:L27 C63:L64 D62:L62 D60:L60 C56:L57 D55:L55 D53:L53 C49:L50 D48:L48 D46:L46 C42:L43 D41:L41 D39:L39 C35:L36 D34:L34 D32:L32 C5:L8" numberStoredAsText="1"/>
+    <ignoredError sqref="C2:L2 C12:L12 D3:L4 C10 D11:L11 C14:L15 D13:L13 C19:L19 D18:L18 C61:L61 D20:L20 C21:L22 C26:L26 C33:L33 C40:L40 C47:L47 C54:L54 D25:L25 C28:L29 D27:L27 C63:L64 D62:L62 D60:L60 C56:L57 D55:L55 D53:L53 C49:L50 D48:L48 D46:L46 C42:L43 D41:L41 D39:L39 C35:L36 D34:L34 D32:L32 C5:L8 E10:L10" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>